<commit_message>
Fix al error del texto de la descripcion y justificacion
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -93,19 +93,25 @@
     <t>Justificación</t>
   </si>
   <si>
+    <t xml:space="preserve"> asdasd asdasd</t>
+  </si>
+  <si>
+    <t>asdasd
+asdasd
+asdasd</t>
+  </si>
+  <si>
     <t>asdasd</t>
   </si>
   <si>
-    <t>dasdasdashdasuihdauishdaisdasdasdasddasdasdashdasuihdauishdaisdasdasdasddasdasdashdasuihdauishdaisdasdasdasddasdasdashdasuihdauishdaisdasdasdasddasdasdashdasuihdauishdaisdasdasdasd</t>
-  </si>
-  <si>
-    <t>dasdasdashdasuihdauishdaisdasdasdasddasdasdashdasuihdauishdaisdasdasdasddasdasdashdasuihdauishdaisdasdasdasddasdasdashdasuihdauishdaisdasdasdasd</t>
-  </si>
-  <si>
-    <t>dasdasdashdasuihdauishdaisdasdasdasddasdasdashdasuihdauishdaisdasdasdasddasdasdashdasuihdauishdaisdasdasdasd</t>
-  </si>
-  <si>
-    <t>dasdasdashdasuihdauishdaisdasdasdasddasdasdashdasuihdauishdaisdasdasdasd</t>
+    <t>asdasd
+asdasd
+asdasd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+asdasdasdasdasdasd
+</t>
   </si>
 </sst>
 </file>
@@ -141,8 +147,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A13:A15"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -516,7 +525,7 @@
     </row>
     <row r="10">
       <c r="A10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
@@ -541,47 +550,44 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13">
+    <row r="13" ht="75" customHeight="true">
+      <c r="A13" s="1">
         <v>1</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C13" t="s">
+    </row>
+    <row r="14" ht="27" customHeight="true">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14">
+      <c r="C14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" ht="51" customHeight="true">
+      <c r="A15" s="1">
         <v>1</v>
       </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C15" t="s">
-        <v>28</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="3">
     <mergeCell ref="A1:A5"/>
     <mergeCell ref="B1:B5"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Simplifica la UI del RequestForm
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="true" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Imagen</t>
   </si>
@@ -93,17 +93,38 @@
     <t>Justificación</t>
   </si>
   <si>
-    <t>asdasdasdasd
-RowRequest</t>
-  </si>
-  <si>
-    <t>asdasd</t>
-  </si>
-  <si>
-    <t>aasdasd</t>
-  </si>
-  <si>
-    <t>asdasda</t>
+    <t>asdasdasd
+asdasdasd</t>
+  </si>
+  <si>
+    <t>asdasdasdasdasdasdasdasdasdasdasdasdasdasdasd
+asdasdasd
+asdasdasd
+asdasdasd</t>
+  </si>
+  <si>
+    <t>asdasdasd asdasdasd</t>
+  </si>
+  <si>
+    <t>asdasdasd
+asdasdasd</t>
+  </si>
+  <si>
+    <t>una pcgaymer</t>
+  </si>
+  <si>
+    <t>asdasdasd 
+asdasd
+asdasd</t>
+  </si>
+  <si>
+    <t>asdasdasdasdasdasd
+asdasdasd</t>
+  </si>
+  <si>
+    <t>asdasdasdasdasdasd asdasdasd
+asdasdasd
+asdasdasd</t>
   </si>
 </sst>
 </file>
@@ -162,7 +183,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -207,7 +228,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -242,7 +263,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -424,13 +445,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A13:A15"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
+    <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col customWidth="true" max="1" min="1" width="30"/>
     <col customWidth="true" max="2" min="2" width="62"/>
@@ -542,34 +561,35 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" ht="39" customHeight="true">
+    <row r="13" ht="87" customHeight="true">
       <c r="A13" s="1">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" ht="27" customHeight="true">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" ht="63" customHeight="true">
       <c r="A14" s="1">
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" ht="51" customHeight="true"/>
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A1:A5"/>
     <mergeCell ref="B1:B5"/>
     <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Stack todas las solicitudes
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Imagen</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Fecha:</t>
   </si>
   <si>
-    <t>31/01/2025</t>
+    <t>01/02/2025</t>
   </si>
   <si>
     <t>Para:</t>
@@ -93,38 +93,25 @@
     <t>Justificación</t>
   </si>
   <si>
-    <t>asdasdasd
-asdasdasd</t>
-  </si>
-  <si>
-    <t>asdasdasdasdasdasdasdasdasdasdasdasdasdasdasd
-asdasdasd
-asdasdasd
-asdasdasd</t>
-  </si>
-  <si>
-    <t>asdasdasd asdasdasd</t>
-  </si>
-  <si>
-    <t>asdasdasd
-asdasdasd</t>
-  </si>
-  <si>
-    <t>una pcgaymer</t>
-  </si>
-  <si>
-    <t>asdasdasd 
-asdasd
-asdasd</t>
-  </si>
-  <si>
-    <t>asdasdasdasdasdasd
-asdasdasd</t>
-  </si>
-  <si>
-    <t>asdasdasdasdasdasd asdasdasd
-asdasdasd
-asdasdasd</t>
+    <t>asdasda</t>
+  </si>
+  <si>
+    <t>asdasd</t>
+  </si>
+  <si>
+    <t>pedro</t>
+  </si>
+  <si>
+    <t>dasdasdasd</t>
+  </si>
+  <si>
+    <t>dasdasd</t>
+  </si>
+  <si>
+    <t>asdasdasd</t>
+  </si>
+  <si>
+    <t>ghjghjghj</t>
   </si>
 </sst>
 </file>
@@ -502,36 +489,29 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-    </row>
+    <row r="6"/>
     <row r="7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10">
@@ -539,57 +519,211 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="b">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s">
+    <row r="13">
+      <c r="A13" t="s">
         <v>21</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" ht="87" customHeight="true">
-      <c r="A13" s="1">
-        <v>1</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    <row r="14" ht="27" customHeight="true">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15"/>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="b">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="b">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="b">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" ht="27" customHeight="true">
+      <c r="A23" s="1">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" ht="63" customHeight="true">
-      <c r="A14" s="1">
-        <v>1</v>
-      </c>
-      <c r="B14" s="1" t="s">
+    <row r="24"/>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="b">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="b">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" ht="27" customHeight="true">
+      <c r="A32" s="1">
+        <v>1</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" ht="27" customHeight="true">
+      <c r="A33" s="1">
+        <v>1</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>31</v>
+      <c r="C33" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
     <mergeCell ref="A1:A5"/>
     <mergeCell ref="B1:B5"/>
-    <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Barra para mostrar las hojas de calculo
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -2,19 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="true" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="hoja random" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>SOLICITUD DE MATERIALES / SERVICIOS / EQUIPO</t>
   </si>
@@ -121,8 +122,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,9 +131,8 @@
       <family val="2"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
-      <color/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -187,31 +187,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true" applyAlignment="false">
-      <alignment/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -227,9 +240,9 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 2" descr=""/>
+        <xdr:cNvPr id="2" name="Picture 2"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="false"/>
+          <a:picLocks/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -243,17 +256,19 @@
           <a:off x="0" y="0"/>
           <a:ext cx="0" cy="0"/>
         </a:xfrm>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
         <a:ln/>
       </xdr:spPr>
     </xdr:pic>
-    <xdr:clientData fLocksWithSheet="true" fPrintsWithSheet="true"/>
+    <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -505,24 +520,32 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col customWidth="true" max="1" min="1" width="30"/>
-    <col customWidth="true" max="2" min="2" width="62"/>
-    <col customWidth="true" max="4" min="3" width="20"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="62" customWidth="1"/>
+    <col min="3" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
@@ -532,8 +555,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
-      <c r="B2" s="1"/>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
       <c r="C2" t="s">
         <v>2</v>
       </c>
@@ -541,8 +565,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
-      <c r="B3" s="1"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
       <c r="C3" t="s">
         <v>3</v>
       </c>
@@ -550,8 +575,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4">
-      <c r="B4" s="1"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
       <c r="C4" t="s">
         <v>4</v>
       </c>
@@ -559,8 +585,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5">
-      <c r="B5" s="1"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
       <c r="C5" t="s">
         <v>5</v>
       </c>
@@ -568,18 +595,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6"/>
-    <row r="7">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -587,7 +613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -595,7 +621,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="b">
         <v>1</v>
       </c>
@@ -603,7 +629,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="b">
         <v>1</v>
       </c>
@@ -611,7 +637,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="b">
         <v>0</v>
       </c>
@@ -619,42 +645,41 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" ht="27" customHeight="true">
-      <c r="A14" s="4">
-        <v>1</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15"/>
-    <row r="16">
-      <c r="A16" s="2" t="s">
+      <c r="D14" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -662,7 +687,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -670,7 +695,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="b">
         <v>0</v>
       </c>
@@ -678,7 +703,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="b">
         <v>1</v>
       </c>
@@ -686,7 +711,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="b">
         <v>1</v>
       </c>
@@ -694,54 +719,53 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" ht="27" customHeight="true">
-      <c r="A23" s="4">
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
         <v>3</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" ht="27" customHeight="true">
-      <c r="A24" s="4">
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
         <v>5</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25"/>
-    <row r="26">
-      <c r="A26" s="2" t="s">
+      <c r="D24" s="7"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -749,7 +773,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -757,7 +781,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="b">
         <v>1</v>
       </c>
@@ -765,7 +789,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="b">
         <v>1</v>
       </c>
@@ -773,7 +797,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="b">
         <v>1</v>
       </c>
@@ -781,55 +805,70 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" ht="27" customHeight="true">
-      <c r="A33" s="4">
-        <v>1</v>
-      </c>
-      <c r="B33" s="4" t="s">
+      <c r="D32" s="6"/>
+    </row>
+    <row r="33" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>1</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="4"/>
-    </row>
-    <row r="34" ht="27" customHeight="true">
-      <c r="A34" s="4">
+      <c r="D33" s="7"/>
+    </row>
+    <row r="34" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
         <v>2</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="4"/>
+      <c r="D34" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
     <mergeCell ref="A1:A5"/>
     <mergeCell ref="B1:B5"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
CRD falta la habilidad de actualizar los registros
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="true" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>SOLICITUD DE MATERIALES / SERVICIOS / EQUIPO</t>
   </si>
@@ -117,13 +117,25 @@
   </si>
   <si>
     <t>Otra Justificación</t>
+  </si>
+  <si>
+    <t>02/02/2025</t>
+  </si>
+  <si>
+    <t>Prueba</t>
+  </si>
+  <si>
+    <t>PruebaPruebaPruebaPruebaPrueba</t>
+  </si>
+  <si>
+    <t>PruebaPruebaPruebaPrueba</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,8 +143,15 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="11"/>
+      <color/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -187,31 +206,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -268,7 +290,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -532,18 +554,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="62" customWidth="1"/>
-    <col min="3" max="4" width="20" customWidth="1"/>
+    <col customWidth="true" max="1" min="1" width="30"/>
+    <col customWidth="true" max="2" min="2" width="62"/>
+    <col customWidth="true" max="4" min="3" width="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -555,7 +577,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" t="s">
@@ -565,7 +587,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" t="s">
@@ -575,7 +597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" t="s">
@@ -585,7 +607,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" t="s">
@@ -595,7 +617,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6"/>
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -605,7 +628,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -613,7 +636,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -621,7 +644,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" t="b">
         <v>1</v>
       </c>
@@ -629,7 +652,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" t="b">
         <v>1</v>
       </c>
@@ -637,7 +660,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" t="b">
         <v>0</v>
       </c>
@@ -645,7 +668,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -657,7 +680,7 @@
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="27" customHeight="true">
       <c r="A14" s="3">
         <v>1</v>
       </c>
@@ -669,7 +692,8 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15"/>
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -679,7 +703,7 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -687,7 +711,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -695,7 +719,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" t="b">
         <v>0</v>
       </c>
@@ -703,7 +727,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4">
       <c r="A20" t="b">
         <v>1</v>
       </c>
@@ -711,7 +735,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4">
       <c r="A21" t="b">
         <v>1</v>
       </c>
@@ -719,7 +743,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -731,7 +755,7 @@
       </c>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="27" customHeight="true">
       <c r="A23" s="3">
         <v>3</v>
       </c>
@@ -743,7 +767,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="27" customHeight="true">
       <c r="A24" s="3">
         <v>5</v>
       </c>
@@ -755,7 +779,8 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25"/>
+    <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
         <v>11</v>
       </c>
@@ -765,7 +790,7 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -773,7 +798,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -781,7 +806,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4">
       <c r="A29" t="b">
         <v>1</v>
       </c>
@@ -789,7 +814,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4">
       <c r="A30" t="b">
         <v>1</v>
       </c>
@@ -797,7 +822,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4">
       <c r="A31" t="b">
         <v>1</v>
       </c>
@@ -805,7 +830,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
         <v>20</v>
       </c>
@@ -817,7 +842,7 @@
       </c>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="27" customHeight="true">
       <c r="A33" s="3">
         <v>1</v>
       </c>
@@ -829,7 +854,7 @@
       </c>
       <c r="D33" s="7"/>
     </row>
-    <row r="34" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="27" customHeight="true">
       <c r="A34" s="3">
         <v>2</v>
       </c>
@@ -841,8 +866,83 @@
       </c>
       <c r="D34" s="7"/>
     </row>
+    <row r="35"/>
+    <row r="36">
+      <c r="A36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="b">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="b">
+        <v>0</v>
+      </c>
+      <c r="B40" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="b">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="8"/>
+    </row>
+    <row r="43" ht="27" customHeight="true">
+      <c r="A43" s="3">
+        <v>1</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C32:D32"/>
@@ -853,6 +953,8 @@
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Cambiar de sheets y abrir el excel
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>SOLICITUD DE MATERIALES / SERVICIOS / EQUIPO</t>
   </si>
@@ -129,6 +129,15 @@
   </si>
   <si>
     <t>PruebaPruebaPruebaPrueba</t>
+  </si>
+  <si>
+    <t>asdasd</t>
+  </si>
+  <si>
+    <t>asdasda</t>
+  </si>
+  <si>
+    <t>sdasdasd</t>
   </si>
 </sst>
 </file>
@@ -285,6 +294,48 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1009650</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 2" descr=""/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="false"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect"/>
+        <a:ln/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="true" fPrintsWithSheet="true"/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
@@ -969,8 +1020,143 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col customWidth="true" max="1" min="1" width="30"/>
+    <col customWidth="true" max="2" min="2" width="62"/>
+    <col customWidth="true" max="4" min="3" width="20"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" s="5"/>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="5"/>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="5"/>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="5"/>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6"/>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="b">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" ht="27" customHeight="true">
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A5"/>
+    <mergeCell ref="B1:B5"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>